<commit_message>
Added another tab called Another Tab
</commit_message>
<xml_diff>
--- a/BYOL4PAASv3.xlsx
+++ b/BYOL4PAASv3.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\Cloud Team\Oracle Public Cloud Offerings\Business Cases for Sales Use Cases\Example BCs excel files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\BMOLNAR\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6510" firstSheet="5" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6800" firstSheet="5" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Impact of Commitment" sheetId="3" r:id="rId1"/>
@@ -18,9 +18,10 @@
     <sheet name="BYOL PAASvsIAAS" sheetId="7" r:id="rId4"/>
     <sheet name="PAAS List Price Change" sheetId="4" r:id="rId5"/>
     <sheet name="PAAS vs On Premise" sheetId="5" r:id="rId6"/>
-    <sheet name="DBEE On Premise list price" sheetId="6" r:id="rId7"/>
+    <sheet name="Another tab" sheetId="8" r:id="rId7"/>
+    <sheet name="DBEE On Premise list price" sheetId="6" r:id="rId8"/>
   </sheets>
-  <calcPr calcId="171027" concurrentCalc="0"/>
+  <calcPr calcId="171027"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -30,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="443" uniqueCount="187">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="444" uniqueCount="188">
   <si>
     <t>Comparing PAAS Options and Costs</t>
   </si>
@@ -893,6 +894,9 @@
   <si>
     <t>vs New lic.</t>
   </si>
+  <si>
+    <t>Another tab to master</t>
+  </si>
 </sst>
 </file>
 
@@ -1352,10 +1356,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
@@ -1451,7 +1455,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{3B2DC663-EEFB-4C8C-9EE8-3135452E5B74}" type="CELLRANGE">
+                    <a:fld id="{685EC733-E930-4133-9178-6A6A0790301A}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1485,7 +1489,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{6D6F8AA6-6E9B-4CFC-BBC3-E08A9C285D96}" type="CELLRANGE">
+                    <a:fld id="{2E3B67B7-747E-4DAA-94C4-A8A19529AE88}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -4846,7 +4850,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{40CC31C2-1590-4DAA-8656-18538FC32C09}" type="CELLRANGE">
+                    <a:fld id="{DC9810DB-7E98-4479-BEDE-B731BD1900EA}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -4880,7 +4884,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{275009A2-6EDA-4B48-B8BB-5BAE09A7BD3A}" type="CELLRANGE">
+                    <a:fld id="{F393CB14-D400-4F7E-91F0-322DD24438DB}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -4914,7 +4918,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{DFA749A1-F01E-4BD4-8436-FB7A5DA561EF}" type="CELLRANGE">
+                    <a:fld id="{FFC58972-2C33-41AF-9872-C6A570014979}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -4948,7 +4952,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{6E322C18-4BE6-4279-9C3D-C0019827BED3}" type="CELLRANGE">
+                    <a:fld id="{CD2C4828-3221-48F5-8440-067157F1FA74}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -4982,7 +4986,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{D162535F-56B5-415B-8E29-776104585030}" type="CELLRANGE">
+                    <a:fld id="{8BD8BA0E-5706-41E8-9C72-A2186A038BA9}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -5205,7 +5209,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{C69D5E2A-12F1-4B76-818C-1E65FD4309E5}" type="VALUE">
+                    <a:fld id="{3E176670-A08D-4BD6-8A5E-C911DD4A47A7}" type="VALUE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[VALUE]</a:t>
@@ -5239,7 +5243,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{F0C62490-5874-443F-AA47-E606DF761DD2}" type="VALUE">
+                    <a:fld id="{D14C7917-9237-495E-BFBA-341E1D2D246C}" type="VALUE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[VALUE]</a:t>
@@ -5273,7 +5277,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{8E26FE71-1722-42CA-A83B-BC3A9B3EC5A1}" type="VALUE">
+                    <a:fld id="{2CFE3187-31C9-4F41-A766-7F495850CBA3}" type="VALUE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[VALUE]</a:t>
@@ -5307,7 +5311,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{312BF521-CF73-4420-8EC2-020B770065F2}" type="VALUE">
+                    <a:fld id="{76E4DDED-7A40-48BE-B612-90538B1B2FAF}" type="VALUE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[VALUE]</a:t>
@@ -5341,7 +5345,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{E1D947B7-EC46-4C67-8F79-9027768CC87A}" type="VALUE">
+                    <a:fld id="{A8AAECA3-5EF5-4D2D-B7C6-C95ED9C263CE}" type="VALUE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[VALUE]</a:t>
@@ -6449,7 +6453,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{7EEB2B21-EF00-4AD2-BA40-DD981B502E62}" type="CELLRANGE">
+                    <a:fld id="{42CC09A8-4601-4D5A-BF07-47FCE8EED7DB}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -6483,7 +6487,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{5D69723D-5273-4F9B-BFB8-6834D15AD8B0}" type="CELLRANGE">
+                    <a:fld id="{13904854-320E-4DB0-85B4-19330F9925FF}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -7165,7 +7169,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{966CA98F-D6DF-4938-80AB-99293469A9C2}" type="CELLRANGE">
+                    <a:fld id="{A3EB1663-2C73-47BA-B289-059FA9B090C9}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -7199,7 +7203,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{9CEE25C8-EA92-48B5-8077-C2E52ADB7A42}" type="CELLRANGE">
+                    <a:fld id="{E7E337D3-5EB0-4AF7-A6F9-CC98C031B69A}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -7233,7 +7237,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{8F6E84F8-56EF-419E-B1CE-D2BD713505FE}" type="CELLRANGE">
+                    <a:fld id="{F88B5B71-FF25-4B79-871F-2073A2DC1D2C}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -7267,7 +7271,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{F95DDADE-0ABC-4F2F-94D0-1228F3503091}" type="CELLRANGE">
+                    <a:fld id="{B1B9BF3F-EC28-4B81-801F-B9067DEF51F2}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -7301,7 +7305,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{1A178189-CAA3-4844-9E60-3C7262E531F9}" type="CELLRANGE">
+                    <a:fld id="{C0663DA4-64C1-4BC5-9A20-29BCDBC79D8C}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -7524,7 +7528,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{507B330A-B0AC-44BF-8866-402CEFABECBF}" type="VALUE">
+                    <a:fld id="{A8160516-0FBF-4551-8ADE-67543C115F92}" type="VALUE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[VALUE]</a:t>
@@ -7558,7 +7562,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{ACA84B75-EE3E-4136-B2B4-CAF10022D7C0}" type="VALUE">
+                    <a:fld id="{99D1B418-45C5-43A0-B5BA-2C1331D9D137}" type="VALUE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[VALUE]</a:t>
@@ -7592,7 +7596,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{0A83F372-9161-46DF-BDDA-0FAE96132847}" type="VALUE">
+                    <a:fld id="{DC8959E4-2186-44C6-B175-A0A3148094DF}" type="VALUE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[VALUE]</a:t>
@@ -7626,7 +7630,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{D42202D7-6359-4132-AF26-D427D433F7B7}" type="VALUE">
+                    <a:fld id="{7F83A05B-A30A-473D-B47C-DBEAD15F360D}" type="VALUE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[VALUE]</a:t>
@@ -7660,7 +7664,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{68B320EB-BF83-4949-8EB4-1D6E88154B95}" type="VALUE">
+                    <a:fld id="{9C51323C-70A8-46B2-98A7-32243122BA3B}" type="VALUE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[VALUE]</a:t>
@@ -8492,7 +8496,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{5AB7E4DC-B031-4C29-9030-373D01F24243}" type="CELLRANGE">
+                    <a:fld id="{FBCF4EE0-0A5F-4A41-83BE-E0D48E94383D}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -8526,7 +8530,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{D80201AC-FCD2-492E-BB45-5877C87CE387}" type="CELLRANGE">
+                    <a:fld id="{97B303AF-B0D4-438B-B385-D9854C634A4B}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -8560,7 +8564,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{C0A4A6EA-D3C8-4010-9CA4-B8C79CFB87EA}" type="CELLRANGE">
+                    <a:fld id="{FA85F78D-E1CD-4F51-83E0-E2A158405934}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -8594,7 +8598,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{8B97FBA8-BCE3-42E4-B9A1-10B956D86468}" type="CELLRANGE">
+                    <a:fld id="{8C33D678-750F-4E3B-A9BE-38B77B7FDD21}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -8628,7 +8632,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{F24DDB93-7648-4FB9-88E0-A6DC3EB7304A}" type="CELLRANGE">
+                    <a:fld id="{02605125-4156-4E47-A7AD-9BE285EF157D}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -8851,7 +8855,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{B0815C06-7C84-454A-963C-D80DB3FA556A}" type="VALUE">
+                    <a:fld id="{743843B7-E5D0-4989-B8E5-BD7FC942F82C}" type="VALUE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[VALUE]</a:t>
@@ -8885,7 +8889,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{C3C03BFB-D6CE-4956-B236-50CFE3D62AB6}" type="VALUE">
+                    <a:fld id="{AC87E573-240D-4A19-BC66-A1EBEE95AE45}" type="VALUE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[VALUE]</a:t>
@@ -8919,7 +8923,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{9E447821-8D53-47F0-AC5C-4838C2D7A130}" type="VALUE">
+                    <a:fld id="{3391B50F-A6F3-41D1-9DD0-F5C3B8A1B7F6}" type="VALUE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[VALUE]</a:t>
@@ -8953,7 +8957,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{1BE4840D-2092-4578-9F6C-C4AF98DDF1C5}" type="VALUE">
+                    <a:fld id="{BEB41DB7-8BF3-4B36-A016-E5798F83B79F}" type="VALUE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[VALUE]</a:t>
@@ -8987,7 +8991,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{251B9EAA-8E9A-4488-B536-E213ADE876D3}" type="VALUE">
+                    <a:fld id="{8B35BED3-B9E4-450C-A103-93F9AEE8268B}" type="VALUE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[VALUE]</a:t>
@@ -9166,7 +9170,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{3147B9BC-7E91-4F4E-9DC0-A6F725933A81}" type="CELLRANGE">
+                    <a:fld id="{68E95506-7BFF-4F99-BDC6-C0078F7E58E4}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -9200,7 +9204,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{E7C680EC-56EF-403F-8958-9E6FD3B1CD95}" type="CELLRANGE">
+                    <a:fld id="{6CEA6C4D-98C0-4AAA-9D50-C53C03CBD87B}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -9234,7 +9238,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{4AE63EC0-85A0-49EA-8D26-BE02048AB593}" type="CELLRANGE">
+                    <a:fld id="{BD8233E3-704B-4DC6-99F4-EF7756CADD57}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -9268,7 +9272,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{C5928DC4-837A-4A83-B444-438CB30C3697}" type="CELLRANGE">
+                    <a:fld id="{7ED0512A-0F09-499B-A658-31AE4BBFD939}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -9302,7 +9306,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{D7B4976C-C962-41D1-8138-CE10467AFFB6}" type="CELLRANGE">
+                    <a:fld id="{BEA6B99A-9D26-4CB9-B650-8413D79B692C}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -9876,7 +9880,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{F1856C0B-8E50-4154-B58C-F5D356F01572}" type="CELLRANGE">
+                    <a:fld id="{DD89E0B2-1431-4AB0-A4D9-40549FEF6BA8}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -9910,7 +9914,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{94B02C95-F5BE-4DA2-A756-365B2B3431F5}" type="CELLRANGE">
+                    <a:fld id="{7E681533-A3A8-4F85-BA2F-2260278E932A}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -9944,7 +9948,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{EE764C51-9718-4FF8-BF10-B07C86756634}" type="CELLRANGE">
+                    <a:fld id="{5AB46204-52B9-4B42-8920-527C3E5C256A}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -9978,7 +9982,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{AF1464DA-AFB2-4C07-97D7-89553809F59C}" type="CELLRANGE">
+                    <a:fld id="{64F4F91D-9378-4AEE-B4CA-1C1042A426F2}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -10518,7 +10522,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{0A62B11E-158B-41E0-BCF3-ACD06986AB12}" type="CELLRANGE">
+                    <a:fld id="{165A0449-431D-4C73-9818-10B0DDCC182F}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -10552,7 +10556,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{F6480B33-FFF6-4BF7-98DF-9CE3C238CD98}" type="CELLRANGE">
+                    <a:fld id="{B1522502-B9EF-45D7-BD5B-63234559E559}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -11095,7 +11099,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{A1CBF31F-136C-4B4C-A0EF-5DCCBF0A8B5C}" type="CELLRANGE">
+                    <a:fld id="{65FB8D74-763D-4B03-9FE0-B3E217A4D3C9}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -11129,7 +11133,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{232E7E70-24DB-4B53-9E23-1C2F9AA7C173}" type="CELLRANGE">
+                    <a:fld id="{DA50004B-9DAE-48F3-95AC-B4096FA84DFB}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -11163,7 +11167,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{16CA4C40-1A12-4033-92DD-2C360188E9F8}" type="CELLRANGE">
+                    <a:fld id="{6F68207F-F956-4968-BF27-3F41E4B3F004}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -11197,7 +11201,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{2A098694-B6A9-4A3E-89B6-A98A891DF9FF}" type="CELLRANGE">
+                    <a:fld id="{A50741C9-E797-47EB-A764-A54DDB8D3BDF}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -18176,7 +18180,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{6E13C809-9462-4BBF-A098-74138152C7AA}" type="CELLRANGE">
+                    <a:fld id="{16C77C0C-49D4-44EE-B91C-4D4A7D4B8D17}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -18210,7 +18214,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{0F5A0420-3BD2-48DD-8CE0-8AFF16359051}" type="CELLRANGE">
+                    <a:fld id="{E1ACEEAB-E179-4267-AA4C-C684E2E2E12A}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -18244,7 +18248,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{DD85965D-E000-4832-90F2-03E3E45FACB8}" type="CELLRANGE">
+                    <a:fld id="{65501166-6299-435D-ADD6-B6A151643CEA}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -18278,7 +18282,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{68BA14CB-5689-4917-B869-5DE1E1BF9D47}" type="CELLRANGE">
+                    <a:fld id="{CBAB81FC-E7FA-4E0F-B34D-95EB0CB0456D}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -18891,7 +18895,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{70A997B4-65B2-460D-BE0D-9125BBBE6F87}" type="CELLRANGE">
+                    <a:fld id="{4E157F75-DB27-40C4-A3B6-6CFDCF032750}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -18940,7 +18944,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{B123DD0F-FDE1-4E08-A10C-D7453F2160CA}" type="CELLRANGE">
+                    <a:fld id="{297811BF-4A4C-4690-8A66-8EB335E25FE8}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -19517,7 +19521,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{47156D11-2D53-4C9A-9B80-A37BCA2484DF}" type="CELLRANGE">
+                    <a:fld id="{ECAA71D0-AEC6-4C0E-ACCC-C074578A4637}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -19566,7 +19570,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{1B3B4F64-9AE3-4B5B-A96A-5ABCD82F37F9}" type="CELLRANGE">
+                    <a:fld id="{D462EF07-5AB5-4E96-A04C-170E1D72614B}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -39518,7 +39522,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:X131"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A62" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A62" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="A62" sqref="A62"/>
     </sheetView>
   </sheetViews>
@@ -39538,37 +39542,37 @@
       <c r="A1" s="46" t="s">
         <v>137</v>
       </c>
-      <c r="O1" s="56" t="s">
+      <c r="O1" s="57" t="s">
         <v>185</v>
       </c>
-      <c r="P1" s="56"/>
-      <c r="Q1" s="56"/>
-      <c r="R1" s="56"/>
-      <c r="S1" s="56"/>
-      <c r="T1" s="56"/>
-      <c r="U1" s="56"/>
-      <c r="V1" s="56"/>
-      <c r="W1" s="56"/>
-      <c r="X1" s="56"/>
+      <c r="P1" s="57"/>
+      <c r="Q1" s="57"/>
+      <c r="R1" s="57"/>
+      <c r="S1" s="57"/>
+      <c r="T1" s="57"/>
+      <c r="U1" s="57"/>
+      <c r="V1" s="57"/>
+      <c r="W1" s="57"/>
+      <c r="X1" s="57"/>
     </row>
     <row r="2" spans="1:24" x14ac:dyDescent="0.35">
-      <c r="K2" s="56" t="s">
+      <c r="K2" s="57" t="s">
         <v>183</v>
       </c>
-      <c r="L2" s="56"/>
-      <c r="M2" s="56"/>
+      <c r="L2" s="57"/>
+      <c r="M2" s="57"/>
       <c r="O2" s="55"/>
-      <c r="P2" s="56" t="s">
+      <c r="P2" s="57" t="s">
         <v>183</v>
       </c>
-      <c r="Q2" s="56"/>
-      <c r="R2" s="56"/>
-      <c r="U2" s="56" t="s">
+      <c r="Q2" s="57"/>
+      <c r="R2" s="57"/>
+      <c r="U2" s="57" t="s">
         <v>184</v>
       </c>
-      <c r="V2" s="56"/>
-      <c r="W2" s="56"/>
-      <c r="X2" s="56"/>
+      <c r="V2" s="57"/>
+      <c r="W2" s="57"/>
+      <c r="X2" s="57"/>
     </row>
     <row r="3" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A3" s="6"/>
@@ -39576,18 +39580,18 @@
       <c r="C3" s="6"/>
       <c r="D3" s="6"/>
       <c r="E3" s="6"/>
-      <c r="F3" s="57" t="s">
+      <c r="F3" s="56" t="s">
         <v>133</v>
       </c>
-      <c r="G3" s="57"/>
-      <c r="H3" s="57"/>
+      <c r="G3" s="56"/>
+      <c r="H3" s="56"/>
       <c r="K3" s="5">
         <v>0.5</v>
       </c>
       <c r="L3" s="58">
         <v>0.3</v>
       </c>
-      <c r="M3" s="56"/>
+      <c r="M3" s="57"/>
       <c r="O3" s="58">
         <v>0</v>
       </c>
@@ -40160,11 +40164,11 @@
       <c r="A59" s="6"/>
       <c r="B59" s="6"/>
       <c r="C59" s="6"/>
-      <c r="D59" s="57" t="s">
+      <c r="D59" s="56" t="s">
         <v>133</v>
       </c>
-      <c r="E59" s="57"/>
-      <c r="F59" s="57"/>
+      <c r="E59" s="56"/>
+      <c r="F59" s="56"/>
       <c r="I59" s="54">
         <f>I58*0.7</f>
         <v>242488.25999999998</v>
@@ -40315,11 +40319,11 @@
       <c r="A67" s="6"/>
       <c r="B67" s="6"/>
       <c r="C67" s="6"/>
-      <c r="D67" s="57" t="s">
+      <c r="D67" s="56" t="s">
         <v>133</v>
       </c>
-      <c r="E67" s="57"/>
-      <c r="F67" s="57"/>
+      <c r="E67" s="56"/>
+      <c r="F67" s="56"/>
     </row>
     <row r="68" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A68" s="6"/>
@@ -40728,11 +40732,11 @@
       <c r="A96" s="6"/>
       <c r="B96" s="6"/>
       <c r="C96" s="6"/>
-      <c r="D96" s="57" t="s">
+      <c r="D96" s="56" t="s">
         <v>133</v>
       </c>
-      <c r="E96" s="57"/>
-      <c r="F96" s="57"/>
+      <c r="E96" s="56"/>
+      <c r="F96" s="56"/>
     </row>
     <row r="97" spans="1:9" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A97" s="6"/>
@@ -40858,11 +40862,11 @@
       <c r="A104" s="6"/>
       <c r="B104" s="6"/>
       <c r="C104" s="6"/>
-      <c r="D104" s="57" t="s">
+      <c r="D104" s="56" t="s">
         <v>133</v>
       </c>
-      <c r="E104" s="57"/>
-      <c r="F104" s="57"/>
+      <c r="E104" s="56"/>
+      <c r="F104" s="56"/>
     </row>
     <row r="105" spans="1:9" ht="29" x14ac:dyDescent="0.35">
       <c r="A105" s="6"/>
@@ -41287,11 +41291,6 @@
     </row>
   </sheetData>
   <mergeCells count="14">
-    <mergeCell ref="D67:F67"/>
-    <mergeCell ref="D96:F96"/>
-    <mergeCell ref="D104:F104"/>
-    <mergeCell ref="K2:M2"/>
-    <mergeCell ref="L3:M3"/>
     <mergeCell ref="P2:R2"/>
     <mergeCell ref="F3:H3"/>
     <mergeCell ref="D59:F59"/>
@@ -41301,6 +41300,11 @@
     <mergeCell ref="W3:X3"/>
     <mergeCell ref="O3:P3"/>
     <mergeCell ref="Q3:R3"/>
+    <mergeCell ref="D67:F67"/>
+    <mergeCell ref="D96:F96"/>
+    <mergeCell ref="D104:F104"/>
+    <mergeCell ref="K2:M2"/>
+    <mergeCell ref="L3:M3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -41309,6 +41313,24 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>187</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I32"/>
   <sheetViews>

</xml_diff>